<commit_message>
12 month increment working now
</commit_message>
<xml_diff>
--- a/chart_config.xlsx
+++ b/chart_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13584" windowHeight="4476" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="4470" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="panels" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>WTI-F</t>
   </si>
@@ -85,19 +85,10 @@
     <t>product_id</t>
   </si>
   <si>
-    <t>Brent-WTI box spread Mar-Apr</t>
-  </si>
-  <si>
-    <t>Brent-WTI box spread Apr-May</t>
-  </si>
-  <si>
-    <t>Brent-WTI box spread May-Jun</t>
-  </si>
-  <si>
-    <t>Brent-WTI box spread Jun-Jul</t>
-  </si>
-  <si>
     <t>expression_id</t>
+  </si>
+  <si>
+    <t>Brent-WTI box spread {front}-{back}</t>
   </si>
 </sst>
 </file>
@@ -415,18 +406,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="39.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -437,47 +428,14 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5">
         <v>5</v>
       </c>
     </row>
@@ -488,18 +446,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -519,7 +477,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -536,66 +494,6 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" t="s">
-        <v>12</v>
-      </c>
-      <c r="F5" t="s">
         <v>14</v>
       </c>
     </row>
@@ -606,21 +504,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
         <v>18</v>
@@ -641,7 +539,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -661,7 +559,7 @@
         <v>202204</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -679,156 +577,6 @@
       </c>
       <c r="G3">
         <v>202204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <f>B2+1</f>
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <f>C2</f>
-        <v>1</v>
-      </c>
-      <c r="D4" t="str">
-        <f>D2</f>
-        <v>BRT-F</v>
-      </c>
-      <c r="E4">
-        <f>E2+1</f>
-        <v>202204</v>
-      </c>
-      <c r="G4">
-        <f>G2+1</f>
-        <v>202205</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <f t="shared" ref="B5:B9" si="0">B3+1</f>
-        <v>2</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ref="C5:D5" si="1">C3</f>
-        <v>-1</v>
-      </c>
-      <c r="D5" t="str">
-        <f t="shared" si="1"/>
-        <v>WTI-F</v>
-      </c>
-      <c r="E5">
-        <f t="shared" ref="E5:E9" si="2">E3+1</f>
-        <v>202204</v>
-      </c>
-      <c r="G5">
-        <f t="shared" ref="G5:G9" si="3">G3+1</f>
-        <v>202205</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <f t="shared" ref="C6:D6" si="4">C4</f>
-        <v>1</v>
-      </c>
-      <c r="D6" t="str">
-        <f t="shared" si="4"/>
-        <v>BRT-F</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="2"/>
-        <v>202205</v>
-      </c>
-      <c r="G6">
-        <f t="shared" si="3"/>
-        <v>202206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="C7">
-        <f t="shared" ref="C7:D7" si="5">C5</f>
-        <v>-1</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="5"/>
-        <v>WTI-F</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="2"/>
-        <v>202205</v>
-      </c>
-      <c r="G7">
-        <f t="shared" si="3"/>
-        <v>202206</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C8">
-        <f t="shared" ref="C8:D8" si="6">C6</f>
-        <v>1</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="6"/>
-        <v>BRT-F</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="2"/>
-        <v>202206</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="3"/>
-        <v>202207</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <f t="shared" ref="C9:D9" si="7">C7</f>
-        <v>-1</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="7"/>
-        <v>WTI-F</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="2"/>
-        <v>202206</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="3"/>
-        <v>202207</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple definitions working now
</commit_message>
<xml_diff>
--- a/chart_config.xlsx
+++ b/chart_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13590" windowHeight="4470" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13596" windowHeight="4476" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="panels" sheetId="3" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>WTI-F</t>
   </si>
@@ -89,6 +89,27 @@
   </si>
   <si>
     <t>Brent-WTI box spread {front}-{back}</t>
+  </si>
+  <si>
+    <t>mt</t>
+  </si>
+  <si>
+    <t>GO-F</t>
+  </si>
+  <si>
+    <t>HO-F</t>
+  </si>
+  <si>
+    <t>extend_tenor</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>extend_count</t>
+  </si>
+  <si>
+    <t>Gasoil-Heating oil  box spread {front}-{back}</t>
   </si>
 </sst>
 </file>
@@ -406,18 +427,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>17</v>
       </c>
@@ -427,8 +448,14 @@
       <c r="C1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -437,6 +464,29 @@
       </c>
       <c r="C2">
         <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -446,18 +496,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -477,7 +527,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -494,6 +544,26 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" t="s">
         <v>14</v>
       </c>
     </row>
@@ -504,19 +574,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>19</v>
       </c>
@@ -539,7 +609,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -559,7 +629,7 @@
         <v>202204</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -576,6 +646,46 @@
         <v>202203</v>
       </c>
       <c r="G3">
+        <v>202204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4">
+        <v>202203</v>
+      </c>
+      <c r="G4">
+        <v>202204</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>-1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5">
+        <v>202203</v>
+      </c>
+      <c r="G5">
         <v>202204</v>
       </c>
     </row>

</xml_diff>